<commit_message>
Add evaluation_results_likert & evaluation_results_mode3
</commit_message>
<xml_diff>
--- a/study/data/stats/generated/stats-adam.xlsx
+++ b/study/data/stats/generated/stats-adam.xlsx
@@ -15,6 +15,8 @@
     <sheet name="a_a_s_f_e_d" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="p_c_f_m_a" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="t_s_e_l_t_s_e_l" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="e_r_l" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="e_r_m" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -797,6 +799,803 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="18" customWidth="1" min="10" max="10"/>
+    <col width="18" customWidth="1" min="11" max="11"/>
+    <col width="18" customWidth="1" min="12" max="12"/>
+    <col width="18" customWidth="1" min="13" max="13"/>
+    <col width="18" customWidth="1" min="14" max="14"/>
+    <col width="18" customWidth="1" min="15" max="15"/>
+    <col width="18" customWidth="1" min="16" max="16"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Evaluation Results Mode3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>tag_eval</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-vanilla-mode3-01</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-base-mode3-01</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n"/>
+      <c r="G3" s="2" t="n"/>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-ext-mode3-01</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="n"/>
+      <c r="J3" s="2" t="n"/>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-vanilla4-mode3-01</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-vanilla4o-mode3-01</t>
+        </is>
+      </c>
+      <c r="O3" s="2" t="n"/>
+      <c r="P3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>metric</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="M4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="N4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="O4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>ALL</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>54.01</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3540</v>
+      </c>
+      <c r="E6" t="n">
+        <v>64.08</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3474</v>
+      </c>
+      <c r="H6" t="n">
+        <v>75.78</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2601</v>
+      </c>
+      <c r="K6" t="n">
+        <v>84.51000000000001</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2525</v>
+      </c>
+      <c r="N6" t="n">
+        <v>85.20999999999999</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="P6" t="n">
+        <v>5045</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>cycling</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="D7" t="n">
+        <v>376</v>
+      </c>
+      <c r="E7" t="n">
+        <v>70.56999999999999</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="G7" t="n">
+        <v>367</v>
+      </c>
+      <c r="H7" t="n">
+        <v>75.09999999999999</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J7" t="n">
+        <v>253</v>
+      </c>
+      <c r="K7" t="n">
+        <v>92.94</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="M7" t="n">
+        <v>269</v>
+      </c>
+      <c r="N7" t="n">
+        <v>90.86</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="P7" t="n">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>cycling-logistics</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>83.95</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="D8" t="n">
+        <v>162</v>
+      </c>
+      <c r="E8" t="n">
+        <v>77.22</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="G8" t="n">
+        <v>158</v>
+      </c>
+      <c r="H8" t="n">
+        <v>85.5</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="J8" t="n">
+        <v>131</v>
+      </c>
+      <c r="K8" t="n">
+        <v>78.3</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="M8" t="n">
+        <v>106</v>
+      </c>
+      <c r="N8" t="n">
+        <v>89.19</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="P8" t="n">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>interested</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="D9" t="n">
+        <v>375</v>
+      </c>
+      <c r="E9" t="n">
+        <v>42.55</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="G9" t="n">
+        <v>369</v>
+      </c>
+      <c r="H9" t="n">
+        <v>40.56</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="J9" t="n">
+        <v>249</v>
+      </c>
+      <c r="K9" t="n">
+        <v>67.66</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="M9" t="n">
+        <v>269</v>
+      </c>
+      <c r="N9" t="n">
+        <v>66.23</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="P9" t="n">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>pers-urgency</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>49.07</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="D10" t="n">
+        <v>375</v>
+      </c>
+      <c r="E10" t="n">
+        <v>76.55</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="G10" t="n">
+        <v>371</v>
+      </c>
+      <c r="H10" t="n">
+        <v>81.08</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="J10" t="n">
+        <v>296</v>
+      </c>
+      <c r="K10" t="n">
+        <v>88.84999999999999</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="M10" t="n">
+        <v>269</v>
+      </c>
+      <c r="N10" t="n">
+        <v>87.13</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="P10" t="n">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>tech</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>73.67</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="D11" t="n">
+        <v>376</v>
+      </c>
+      <c r="E11" t="n">
+        <v>82.56999999999999</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="G11" t="n">
+        <v>373</v>
+      </c>
+      <c r="H11" t="n">
+        <v>89.36</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="J11" t="n">
+        <v>329</v>
+      </c>
+      <c r="K11" t="n">
+        <v>87.73</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="M11" t="n">
+        <v>269</v>
+      </c>
+      <c r="N11" t="n">
+        <v>93.66</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="P11" t="n">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>urgency</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>56.38</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="D12" t="n">
+        <v>376</v>
+      </c>
+      <c r="E12" t="n">
+        <v>75.95</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="G12" t="n">
+        <v>370</v>
+      </c>
+      <c r="H12" t="n">
+        <v>81.84999999999999</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J12" t="n">
+        <v>270</v>
+      </c>
+      <c r="K12" t="n">
+        <v>92.54000000000001</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="M12" t="n">
+        <v>268</v>
+      </c>
+      <c r="N12" t="n">
+        <v>93.47</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="P12" t="n">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>work-logistics</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>63.83</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="D13" t="n">
+        <v>376</v>
+      </c>
+      <c r="E13" t="n">
+        <v>66.76000000000001</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="G13" t="n">
+        <v>370</v>
+      </c>
+      <c r="H13" t="n">
+        <v>89.19</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="J13" t="n">
+        <v>259</v>
+      </c>
+      <c r="K13" t="n">
+        <v>91.04000000000001</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="M13" t="n">
+        <v>268</v>
+      </c>
+      <c r="N13" t="n">
+        <v>90.67</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="P13" t="n">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>work-pers</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>31.28</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="D14" t="n">
+        <v>374</v>
+      </c>
+      <c r="E14" t="n">
+        <v>32.95</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G14" t="n">
+        <v>346</v>
+      </c>
+      <c r="H14" t="n">
+        <v>40.11</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J14" t="n">
+        <v>182</v>
+      </c>
+      <c r="K14" t="n">
+        <v>69.52</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M14" t="n">
+        <v>269</v>
+      </c>
+      <c r="N14" t="n">
+        <v>69.34999999999999</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="P14" t="n">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>work-relevant</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>48.94</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="D15" t="n">
+        <v>376</v>
+      </c>
+      <c r="E15" t="n">
+        <v>54.86</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="G15" t="n">
+        <v>370</v>
+      </c>
+      <c r="H15" t="n">
+        <v>74.05</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="J15" t="n">
+        <v>289</v>
+      </c>
+      <c r="K15" t="n">
+        <v>82.16</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="M15" t="n">
+        <v>269</v>
+      </c>
+      <c r="N15" t="n">
+        <v>83.58</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="P15" t="n">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>work-urgency</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>29.14</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="D16" t="n">
+        <v>374</v>
+      </c>
+      <c r="E16" t="n">
+        <v>66.05</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G16" t="n">
+        <v>380</v>
+      </c>
+      <c r="H16" t="n">
+        <v>86.01000000000001</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="J16" t="n">
+        <v>343</v>
+      </c>
+      <c r="K16" t="n">
+        <v>90.70999999999999</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="M16" t="n">
+        <v>269</v>
+      </c>
+      <c r="N16" t="n">
+        <v>90.3</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="P16" t="n">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Percentage of items in the data set that are AGREE (evaluation_agreement_int = 1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Weighted average of Agreement Score, based on evaluation_agreement_int</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Total number of items in data set</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>interpretation</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>This is the aggregated synthetic evaluation of the ML classification for mode 3 evaluations, which use an Agree/Disagree-based evaluation.  An Agreement Score of close to 1 means the ML classifications have been evaluated to be mostly correct, while a score close to 0 means that they have been evaluated as mostly incorrect.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="N3:P3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -30416,4 +31215,1430 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AE23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="18" customWidth="1" min="10" max="10"/>
+    <col width="18" customWidth="1" min="11" max="11"/>
+    <col width="18" customWidth="1" min="12" max="12"/>
+    <col width="18" customWidth="1" min="13" max="13"/>
+    <col width="18" customWidth="1" min="14" max="14"/>
+    <col width="18" customWidth="1" min="15" max="15"/>
+    <col width="18" customWidth="1" min="16" max="16"/>
+    <col width="18" customWidth="1" min="17" max="17"/>
+    <col width="18" customWidth="1" min="18" max="18"/>
+    <col width="18" customWidth="1" min="19" max="19"/>
+    <col width="18" customWidth="1" min="20" max="20"/>
+    <col width="18" customWidth="1" min="21" max="21"/>
+    <col width="18" customWidth="1" min="22" max="22"/>
+    <col width="18" customWidth="1" min="23" max="23"/>
+    <col width="18" customWidth="1" min="24" max="24"/>
+    <col width="18" customWidth="1" min="25" max="25"/>
+    <col width="18" customWidth="1" min="26" max="26"/>
+    <col width="18" customWidth="1" min="27" max="27"/>
+    <col width="18" customWidth="1" min="28" max="28"/>
+    <col width="18" customWidth="1" min="29" max="29"/>
+    <col width="18" customWidth="1" min="30" max="30"/>
+    <col width="18" customWidth="1" min="31" max="31"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Evaluation Results Likert</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>tag_eval</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-vanilla-mode1-01</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" s="2" t="n"/>
+      <c r="F3" s="2" t="n"/>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-vanilla-mode1-02</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n"/>
+      <c r="I3" s="2" t="n"/>
+      <c r="J3" s="2" t="n"/>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-vanilla-mode2-01</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="n"/>
+      <c r="O3" s="2" t="n"/>
+      <c r="P3" s="2" t="n"/>
+      <c r="Q3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-base-mode2-01</t>
+        </is>
+      </c>
+      <c r="R3" s="2" t="n"/>
+      <c r="S3" s="2" t="n"/>
+      <c r="T3" s="2" t="n"/>
+      <c r="U3" s="2" t="n"/>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-vanilla4-mode2-01</t>
+        </is>
+      </c>
+      <c r="W3" s="2" t="n"/>
+      <c r="X3" s="2" t="n"/>
+      <c r="Y3" s="2" t="n"/>
+      <c r="Z3" s="2" t="n"/>
+      <c r="AA3" s="2" t="inlineStr">
+        <is>
+          <t>phase2-vanilla4o-mode2-01</t>
+        </is>
+      </c>
+      <c r="AB3" s="2" t="n"/>
+      <c r="AC3" s="2" t="n"/>
+      <c r="AD3" s="2" t="n"/>
+      <c r="AE3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>metric</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>mean_likert</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>stddev</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>mean_likert</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>stddev</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>mean_likert</t>
+        </is>
+      </c>
+      <c r="M4" s="2" t="inlineStr">
+        <is>
+          <t>stddev</t>
+        </is>
+      </c>
+      <c r="N4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="O4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="Q4" s="2" t="inlineStr">
+        <is>
+          <t>mean_likert</t>
+        </is>
+      </c>
+      <c r="R4" s="2" t="inlineStr">
+        <is>
+          <t>stddev</t>
+        </is>
+      </c>
+      <c r="S4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="T4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="U4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="V4" s="2" t="inlineStr">
+        <is>
+          <t>mean_likert</t>
+        </is>
+      </c>
+      <c r="W4" s="2" t="inlineStr">
+        <is>
+          <t>stddev</t>
+        </is>
+      </c>
+      <c r="X4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="Y4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="Z4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="AA4" s="2" t="inlineStr">
+        <is>
+          <t>mean_likert</t>
+        </is>
+      </c>
+      <c r="AB4" s="2" t="inlineStr">
+        <is>
+          <t>stddev</t>
+        </is>
+      </c>
+      <c r="AC4" s="2" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="AD4" s="2" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="AE4" s="2" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>ALL</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D6" t="n">
+        <v>73.66</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2160</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I6" t="n">
+        <v>57.02</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4397</v>
+      </c>
+      <c r="L6" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N6" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="P6" t="n">
+        <v>2172</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>4.44</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S6" t="n">
+        <v>84.64</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="U6" t="n">
+        <v>957</v>
+      </c>
+      <c r="V6" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="W6" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X6" t="n">
+        <v>83.15000000000001</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>2232</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>4.56</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>89.37</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>3622</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>cycling</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D7" t="n">
+        <v>94.76000000000001</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F7" t="n">
+        <v>229</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I7" t="n">
+        <v>90.65000000000001</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="K7" t="n">
+        <v>460</v>
+      </c>
+      <c r="L7" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N7" t="n">
+        <v>70.56</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="P7" t="n">
+        <v>231</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>4.66</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S7" t="n">
+        <v>91.18000000000001</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="U7" t="n">
+        <v>102</v>
+      </c>
+      <c r="V7" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="W7" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X7" t="n">
+        <v>92.83</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>237</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>4.71</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>92.73</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>cycling-logistics</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D8" t="n">
+        <v>91.75</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="F8" t="n">
+        <v>97</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I8" t="n">
+        <v>90.81999999999999</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="K8" t="n">
+        <v>196</v>
+      </c>
+      <c r="L8" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N8" t="n">
+        <v>49.48</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="P8" t="n">
+        <v>97</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S8" t="n">
+        <v>88.64</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="U8" t="n">
+        <v>44</v>
+      </c>
+      <c r="V8" t="n">
+        <v>4.51</v>
+      </c>
+      <c r="W8" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X8" t="n">
+        <v>86.73</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>98</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>89.81</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>interested</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D9" t="n">
+        <v>68.56</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="F9" t="n">
+        <v>229</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I9" t="n">
+        <v>65.15000000000001</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="K9" t="n">
+        <v>462</v>
+      </c>
+      <c r="L9" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N9" t="n">
+        <v>39.39</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="P9" t="n">
+        <v>231</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S9" t="n">
+        <v>60.78</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="U9" t="n">
+        <v>102</v>
+      </c>
+      <c r="V9" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="W9" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X9" t="n">
+        <v>63.29</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>237</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>74.03</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>pers-urgency</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D10" t="n">
+        <v>61.57</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="F10" t="n">
+        <v>229</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I10" t="n">
+        <v>42.76</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="K10" t="n">
+        <v>463</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N10" t="n">
+        <v>19.91</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="P10" t="n">
+        <v>231</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>4.73</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S10" t="n">
+        <v>92.23</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="U10" t="n">
+        <v>103</v>
+      </c>
+      <c r="V10" t="n">
+        <v>4.47</v>
+      </c>
+      <c r="W10" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X10" t="n">
+        <v>85.23</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>237</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>92.20999999999999</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>tech</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D11" t="n">
+        <v>84.72</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="F11" t="n">
+        <v>229</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I11" t="n">
+        <v>62</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="K11" t="n">
+        <v>471</v>
+      </c>
+      <c r="L11" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N11" t="n">
+        <v>38.1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="P11" t="n">
+        <v>231</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>4.78</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S11" t="n">
+        <v>94.17</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="U11" t="n">
+        <v>103</v>
+      </c>
+      <c r="V11" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="W11" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X11" t="n">
+        <v>89.95999999999999</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>239</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>94.29000000000001</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>urgency</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D12" t="n">
+        <v>64.63</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="F12" t="n">
+        <v>229</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I12" t="n">
+        <v>41.9</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="K12" t="n">
+        <v>463</v>
+      </c>
+      <c r="L12" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N12" t="n">
+        <v>24.68</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="P12" t="n">
+        <v>231</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S12" t="n">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="U12" t="n">
+        <v>102</v>
+      </c>
+      <c r="V12" t="n">
+        <v>4.66</v>
+      </c>
+      <c r="W12" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X12" t="n">
+        <v>90.17</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>234</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>4.73</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>95.31999999999999</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>work-logistics</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D13" t="n">
+        <v>89.08</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="F13" t="n">
+        <v>229</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I13" t="n">
+        <v>68.26000000000001</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K13" t="n">
+        <v>460</v>
+      </c>
+      <c r="L13" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N13" t="n">
+        <v>33.77</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="P13" t="n">
+        <v>231</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>4.81</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S13" t="n">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="U13" t="n">
+        <v>102</v>
+      </c>
+      <c r="V13" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="W13" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X13" t="n">
+        <v>91.14</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>237</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>95.06</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>work-pers</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D14" t="n">
+        <v>59.83</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="F14" t="n">
+        <v>229</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I14" t="n">
+        <v>55.97</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="K14" t="n">
+        <v>461</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N14" t="n">
+        <v>25.55</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="P14" t="n">
+        <v>227</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="R14" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S14" t="n">
+        <v>62.64</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="U14" t="n">
+        <v>91</v>
+      </c>
+      <c r="V14" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="W14" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X14" t="n">
+        <v>64.14</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>237</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>82.08</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>work-relevant</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D15" t="n">
+        <v>68.56</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F15" t="n">
+        <v>229</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I15" t="n">
+        <v>46.22</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="K15" t="n">
+        <v>463</v>
+      </c>
+      <c r="L15" t="n">
+        <v>2.81</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N15" t="n">
+        <v>25.97</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="P15" t="n">
+        <v>231</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S15" t="n">
+        <v>80.58</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="U15" t="n">
+        <v>103</v>
+      </c>
+      <c r="V15" t="n">
+        <v>4.37</v>
+      </c>
+      <c r="W15" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X15" t="n">
+        <v>81.43000000000001</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>237</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>86.48999999999999</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>work-urgency</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="D16" t="n">
+        <v>63.64</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="F16" t="n">
+        <v>231</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="I16" t="n">
+        <v>28.31</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="K16" t="n">
+        <v>498</v>
+      </c>
+      <c r="L16" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="N16" t="n">
+        <v>7.36</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="P16" t="n">
+        <v>231</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>4.47</v>
+      </c>
+      <c r="R16" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="S16" t="n">
+        <v>85.70999999999999</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="U16" t="n">
+        <v>105</v>
+      </c>
+      <c r="V16" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="W16" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="X16" t="n">
+        <v>88.7</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>239</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>4.66</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>91.95</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>mean_likert</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>The mean value of 'evaluation_likert_val' fopr this data</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>stddev</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Standard deviation of mean_likert data</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>agreement_percentage</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Percentage of evaluation_likert_val in the data set that are AGREE, where agreement is considered to be evaluation_likert_val 4 or 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>weighted_agreement_score</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Weighted average of Agreement Score, where evaluation Likert values are assigned a score: 1: 0, 2: 0.25, 3: 0.5, 4: 0.75, 5: 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Total number of items in data set</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>interpretation</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>This is the aggregated synthetic evaluation of the ML classification for modes 1 &amp; 2 evaluations, which use a Likert-based evaluation.  An Agreement Score of close to 1 means the ML classifications have been evaluated to be mostly correct, while a score close to 0 means that they have been evaluated as mostly incorrect.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A1:AE1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>